<commit_message>
changes for BW training; grix mix exploration in ecoinvent
</commit_message>
<xml_diff>
--- a/import_test.xlsx
+++ b/import_test.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rhanes\GitHub\autoBW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7236080B-94C5-4DBC-A891-F74581C0611B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8254568-0B95-4DFB-8CC2-1E5504CF4A4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12735" yWindow="1455" windowWidth="16050" windowHeight="13680" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28860" yWindow="4020" windowWidth="16050" windowHeight="13680" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Create Activities" sheetId="5" r:id="rId1"/>
-    <sheet name="Delete Exchanges" sheetId="3" r:id="rId2"/>
-    <sheet name="Add Exchanges" sheetId="4" r:id="rId3"/>
+    <sheet name="Add Exchanges" sheetId="4" r:id="rId2"/>
+    <sheet name="Delete Exchanges" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="47">
   <si>
     <t>Type</t>
   </si>
@@ -135,12 +135,6 @@
   </si>
   <si>
     <t>electric grid mix</t>
-  </si>
-  <si>
-    <t>new database</t>
-  </si>
-  <si>
-    <t>code from new act</t>
   </si>
   <si>
     <t>04b818d7946b8689c96aaea50d6a076f</t>
@@ -1025,7 +1019,7 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1052,25 +1046,25 @@
         <v>9</v>
       </c>
       <c r="D1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F1" t="s">
         <v>2</v>
       </c>
       <c r="G1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H1" t="s">
         <v>1</v>
       </c>
       <c r="I1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="J1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -1078,13 +1072,13 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" t="s">
         <v>44</v>
-      </c>
-      <c r="C2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D2" t="s">
-        <v>46</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -1105,6 +1099,239 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB2043D1-6EE9-43E0-B324-EF1E0EADF96E}">
+  <dimension ref="A1:P8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="50.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="34" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2">
+        <v>1.5</v>
+      </c>
+      <c r="H2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I3" t="s">
+        <v>3</v>
+      </c>
+      <c r="J3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" t="s">
+        <v>31</v>
+      </c>
+      <c r="G4">
+        <v>0.5</v>
+      </c>
+      <c r="H4" t="s">
+        <v>30</v>
+      </c>
+      <c r="I4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5">
+        <v>0.5</v>
+      </c>
+      <c r="H5" t="s">
+        <v>30</v>
+      </c>
+      <c r="I5" t="s">
+        <v>3</v>
+      </c>
+      <c r="J5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" t="s">
+        <v>45</v>
+      </c>
+      <c r="D8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0948324-ADD0-429A-AD05-3510BCB3C5ED}">
   <dimension ref="A1:Q5"/>
   <sheetViews>
@@ -1221,253 +1448,20 @@
         <v>27</v>
       </c>
       <c r="C5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F5" t="s">
         <v>36</v>
-      </c>
-      <c r="D5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" t="s">
-        <v>37</v>
-      </c>
-      <c r="F5" t="s">
-        <v>38</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB2043D1-6EE9-43E0-B324-EF1E0EADF96E}">
-  <dimension ref="A1:P8"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="28" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="50.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="34" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2">
-        <v>1.5</v>
-      </c>
-      <c r="H2" t="s">
-        <v>5</v>
-      </c>
-      <c r="I2" t="s">
-        <v>3</v>
-      </c>
-      <c r="J2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F3" t="s">
-        <v>26</v>
-      </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-      <c r="H3" t="s">
-        <v>5</v>
-      </c>
-      <c r="I3" t="s">
-        <v>3</v>
-      </c>
-      <c r="J3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C4" t="s">
-        <v>35</v>
-      </c>
-      <c r="D4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" t="s">
-        <v>28</v>
-      </c>
-      <c r="F4" t="s">
-        <v>31</v>
-      </c>
-      <c r="G4">
-        <v>0.5</v>
-      </c>
-      <c r="H4" t="s">
-        <v>30</v>
-      </c>
-      <c r="I4" t="s">
-        <v>3</v>
-      </c>
-      <c r="J4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" t="s">
-        <v>29</v>
-      </c>
-      <c r="F5" t="s">
-        <v>32</v>
-      </c>
-      <c r="G5">
-        <v>0.5</v>
-      </c>
-      <c r="H5" t="s">
-        <v>30</v>
-      </c>
-      <c r="I5" t="s">
-        <v>3</v>
-      </c>
-      <c r="J5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>44</v>
-      </c>
-      <c r="B6" t="s">
-        <v>45</v>
-      </c>
-      <c r="C6" t="s">
-        <v>47</v>
-      </c>
-      <c r="D6" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>44</v>
-      </c>
-      <c r="B7" t="s">
-        <v>45</v>
-      </c>
-      <c r="C7" t="s">
-        <v>47</v>
-      </c>
-      <c r="D7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>44</v>
-      </c>
-      <c r="B8" t="s">
-        <v>45</v>
-      </c>
-      <c r="C8" t="s">
-        <v>47</v>
-      </c>
-      <c r="D8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
adds grid mix notebook and code, data updates
</commit_message>
<xml_diff>
--- a/import_test.xlsx
+++ b/import_test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rhanes\GitHub\autoBW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8254568-0B95-4DFB-8CC2-1E5504CF4A4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFA54E52-C75A-460C-BCBA-5A2FCF210240}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28860" yWindow="4020" windowWidth="16050" windowHeight="13680" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9900" yWindow="1020" windowWidth="16110" windowHeight="12195" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Create Activities" sheetId="5" r:id="rId1"/>
@@ -33,23 +33,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="47">
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>Location</t>
-  </si>
-  <si>
-    <t>Unit</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="47">
   <si>
     <t>US</t>
   </si>
   <si>
-    <t>Technosphere</t>
-  </si>
-  <si>
     <t>kg</t>
   </si>
   <si>
@@ -71,9 +59,6 @@
     <t>Exchange Name</t>
   </si>
   <si>
-    <t>Exchange Amount</t>
-  </si>
-  <si>
     <t>ecoinvent 3.7.1 consequential</t>
   </si>
   <si>
@@ -110,30 +95,9 @@
     <t>0733b2583ae87bebc1bb4a64798ade38</t>
   </si>
   <si>
-    <t>market for cement, pozzolana and fly ash 15-40%</t>
-  </si>
-  <si>
-    <t>bb3986f5f9d6d47b5007c31999d5fe49</t>
-  </si>
-  <si>
     <t>market for electricity, medium voltage</t>
   </si>
   <si>
-    <t>electricity production, wind, 1-3MW turbine, onshore</t>
-  </si>
-  <si>
-    <t>electricity production, solar tower power plant, 20 MW</t>
-  </si>
-  <si>
-    <t>kwh</t>
-  </si>
-  <si>
-    <t>b60b51f62b2020946acd430337b6e585</t>
-  </si>
-  <si>
-    <t>b9d3338d6c3d52b59394179f9fa2b1ff</t>
-  </si>
-  <si>
     <t>electric grid mix</t>
   </si>
   <si>
@@ -146,21 +110,6 @@
     <t>43251df807f82a95b6c475078e4ba12c</t>
   </si>
   <si>
-    <t>Amount</t>
-  </si>
-  <si>
-    <t>Std_dev.</t>
-  </si>
-  <si>
-    <t>Version</t>
-  </si>
-  <si>
-    <t>Code</t>
-  </si>
-  <si>
-    <t>Reference Product</t>
-  </si>
-  <si>
     <t>newdb</t>
   </si>
   <si>
@@ -170,10 +119,61 @@
     <t>2-Methyl pentane, from chemistry, at plant</t>
   </si>
   <si>
-    <t>uuid</t>
-  </si>
-  <si>
-    <t>Activity Database</t>
+    <t>database</t>
+  </si>
+  <si>
+    <t>activity_name</t>
+  </si>
+  <si>
+    <t>reference_product</t>
+  </si>
+  <si>
+    <t>reference_product_amount</t>
+  </si>
+  <si>
+    <t>reference_product_unit</t>
+  </si>
+  <si>
+    <t>std_dev</t>
+  </si>
+  <si>
+    <t>location</t>
+  </si>
+  <si>
+    <t>activity_version</t>
+  </si>
+  <si>
+    <t>activity_code</t>
+  </si>
+  <si>
+    <t>fancy chemical, from a technology, at plant</t>
+  </si>
+  <si>
+    <t>fancy chemical</t>
+  </si>
+  <si>
+    <t>exchange</t>
+  </si>
+  <si>
+    <t>amount</t>
+  </si>
+  <si>
+    <t>unit</t>
+  </si>
+  <si>
+    <t>electricity</t>
+  </si>
+  <si>
+    <t>kWh</t>
+  </si>
+  <si>
+    <t>2-Methyl pentane,  from chemistry, at plant</t>
+  </si>
+  <si>
+    <t>exchange_db</t>
+  </si>
+  <si>
+    <t>2-Methyl pentane, from chemistry</t>
   </si>
 </sst>
 </file>
@@ -1016,81 +1016,124 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{277CB9D4-0D4C-4491-B6C5-72355C9F8902}">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="40" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>2</v>
+      </c>
+      <c r="G2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="H2">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" t="s">
         <v>37</v>
       </c>
-      <c r="F1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="C3" t="s">
         <v>38</v>
       </c>
-      <c r="H1" t="s">
+      <c r="D3">
         <v>1</v>
       </c>
-      <c r="I1" t="s">
-        <v>39</v>
-      </c>
-      <c r="J1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="E3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" t="s">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" t="s">
         <v>42</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
         <v>43</v>
       </c>
-      <c r="D2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2">
-        <v>2</v>
-      </c>
-      <c r="H2" t="s">
-        <v>3</v>
+      <c r="G4" t="s">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0.1</v>
       </c>
     </row>
   </sheetData>
@@ -1100,230 +1143,210 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB2043D1-6EE9-43E0-B324-EF1E0EADF96E}">
-  <dimension ref="A1:P8"/>
+  <dimension ref="A1:M8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="50.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="34" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>10</v>
+        <v>45</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>7</v>
+        <v>39</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>6</v>
+        <v>41</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>0</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>15</v>
+        <v>21</v>
+      </c>
+      <c r="C2" t="s">
+        <v>25</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2">
-        <v>1.5</v>
-      </c>
-      <c r="H2" t="s">
-        <v>5</v>
-      </c>
-      <c r="I2" t="s">
-        <v>3</v>
-      </c>
-      <c r="J2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+      <c r="E2">
+        <v>0.8</v>
+      </c>
+      <c r="F2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="B3" t="s">
         <v>21</v>
       </c>
       <c r="C3" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" t="s">
-        <v>25</v>
+        <v>42</v>
+      </c>
+      <c r="E3">
+        <v>0.1</v>
       </c>
       <c r="F3" t="s">
-        <v>26</v>
-      </c>
-      <c r="G3">
+        <v>43</v>
+      </c>
+      <c r="G3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E4">
+        <v>4</v>
+      </c>
+      <c r="F4" t="s">
+        <v>43</v>
+      </c>
+      <c r="G4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5">
+        <v>0.2</v>
+      </c>
+      <c r="F5" t="s">
         <v>1</v>
       </c>
-      <c r="H3" t="s">
-        <v>5</v>
-      </c>
-      <c r="I3" t="s">
+      <c r="G5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" t="s">
+        <v>46</v>
+      </c>
+      <c r="E6">
+        <v>0.01</v>
+      </c>
+      <c r="F6" t="s">
+        <v>1</v>
+      </c>
+      <c r="G6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" t="s">
+        <v>42</v>
+      </c>
+      <c r="E7">
         <v>3</v>
       </c>
-      <c r="J3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>42</v>
-      </c>
-      <c r="B4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C4" t="s">
-        <v>45</v>
-      </c>
-      <c r="D4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" t="s">
-        <v>28</v>
-      </c>
-      <c r="F4" t="s">
-        <v>31</v>
-      </c>
-      <c r="G4">
-        <v>0.5</v>
-      </c>
-      <c r="H4" t="s">
-        <v>30</v>
-      </c>
-      <c r="I4" t="s">
-        <v>3</v>
-      </c>
-      <c r="J4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>42</v>
-      </c>
-      <c r="B5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C5" t="s">
-        <v>45</v>
-      </c>
-      <c r="D5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" t="s">
-        <v>29</v>
-      </c>
-      <c r="F5" t="s">
-        <v>32</v>
-      </c>
-      <c r="G5">
-        <v>0.5</v>
-      </c>
-      <c r="H5" t="s">
-        <v>30</v>
-      </c>
-      <c r="I5" t="s">
-        <v>3</v>
-      </c>
-      <c r="J5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>42</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="F7" t="s">
         <v>43</v>
       </c>
-      <c r="C6" t="s">
-        <v>45</v>
-      </c>
-      <c r="D6" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>42</v>
-      </c>
-      <c r="B7" t="s">
-        <v>43</v>
-      </c>
-      <c r="C7" t="s">
-        <v>45</v>
-      </c>
-      <c r="D7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="G7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="B8" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C8" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="D8" t="s">
-        <v>13</v>
+        <v>46</v>
+      </c>
+      <c r="E8">
+        <v>0.78</v>
+      </c>
+      <c r="F8" t="s">
+        <v>1</v>
+      </c>
+      <c r="G8" t="s">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1336,7 +1359,7 @@
   <dimension ref="A1:Q5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1351,22 +1374,22 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
@@ -1382,82 +1405,82 @@
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E2" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
         <v>13</v>
       </c>
-      <c r="B3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" t="s">
-        <v>18</v>
-      </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E3" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="F3" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C4" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D4" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E4" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="F4" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="C5" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="D5" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E5" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="F5" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adds on to file IO functionality
</commit_message>
<xml_diff>
--- a/import_test.xlsx
+++ b/import_test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rhanes\GitHub\autoBW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFA54E52-C75A-460C-BCBA-5A2FCF210240}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E216D03C-01F8-44BB-BB93-46F503406219}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9900" yWindow="1020" windowWidth="16110" windowHeight="12195" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29745" yWindow="5175" windowWidth="14760" windowHeight="13785" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Create Activities" sheetId="5" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="46">
   <si>
     <t>US</t>
   </si>
@@ -113,9 +113,6 @@
     <t>newdb</t>
   </si>
   <si>
-    <t>2-Methyl pentane,  from chemistry</t>
-  </si>
-  <si>
     <t>2-Methyl pentane, from chemistry, at plant</t>
   </si>
   <si>
@@ -143,37 +140,37 @@
     <t>activity_version</t>
   </si>
   <si>
+    <t>exchange</t>
+  </si>
+  <si>
+    <t>amount</t>
+  </si>
+  <si>
+    <t>unit</t>
+  </si>
+  <si>
+    <t>kWh</t>
+  </si>
+  <si>
+    <t>exchange_db</t>
+  </si>
+  <si>
+    <t>2-Methyl pentane, from chemistry</t>
+  </si>
+  <si>
+    <t>fancy chemical, at plant</t>
+  </si>
+  <si>
+    <t>fancy chemical, from a technology</t>
+  </si>
+  <si>
+    <t>electricity</t>
+  </si>
+  <si>
     <t>activity_code</t>
   </si>
   <si>
-    <t>fancy chemical, from a technology, at plant</t>
-  </si>
-  <si>
-    <t>fancy chemical</t>
-  </si>
-  <si>
-    <t>exchange</t>
-  </si>
-  <si>
-    <t>amount</t>
-  </si>
-  <si>
-    <t>unit</t>
-  </si>
-  <si>
-    <t>electricity</t>
-  </si>
-  <si>
-    <t>kWh</t>
-  </si>
-  <si>
-    <t>2-Methyl pentane,  from chemistry, at plant</t>
-  </si>
-  <si>
-    <t>exchange_db</t>
-  </si>
-  <si>
-    <t>2-Methyl pentane, from chemistry</t>
+    <t>exchange_code</t>
   </si>
 </sst>
 </file>
@@ -657,10 +654,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1018,14 +1016,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{277CB9D4-0D4C-4491-B6C5-72355C9F8902}">
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="40" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22.5703125" bestFit="1" customWidth="1"/>
@@ -1037,31 +1035,31 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" t="s">
         <v>28</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>29</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>30</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>31</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>32</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>33</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>34</v>
       </c>
-      <c r="H1" t="s">
-        <v>35</v>
-      </c>
       <c r="I1" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -1069,10 +1067,10 @@
         <v>25</v>
       </c>
       <c r="B2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" t="s">
         <v>26</v>
-      </c>
-      <c r="C2" t="s">
-        <v>27</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -1095,10 +1093,10 @@
         <v>25</v>
       </c>
       <c r="B3" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="C3" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -1121,13 +1119,13 @@
         <v>21</v>
       </c>
       <c r="C4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="G4" t="s">
         <v>0</v>
@@ -1145,8 +1143,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB2043D1-6EE9-43E0-B324-EF1E0EADF96E}">
   <dimension ref="A1:M8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1154,35 +1152,41 @@
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="39.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
@@ -1199,7 +1203,7 @@
         <v>25</v>
       </c>
       <c r="D2" t="s">
-        <v>46</v>
+        <v>26</v>
       </c>
       <c r="E2">
         <v>0.8</v>
@@ -1222,13 +1226,13 @@
         <v>25</v>
       </c>
       <c r="D3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E3">
         <v>0.1</v>
       </c>
       <c r="F3" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="G3" t="s">
         <v>0</v>
@@ -1239,19 +1243,19 @@
         <v>25</v>
       </c>
       <c r="B4" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C4" t="s">
         <v>25</v>
       </c>
       <c r="D4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E4">
         <v>4</v>
       </c>
       <c r="F4" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="G4" t="s">
         <v>0</v>
@@ -1262,13 +1266,13 @@
         <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C5" t="s">
         <v>25</v>
       </c>
       <c r="D5" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="E5">
         <v>0.2</v>
@@ -1285,13 +1289,13 @@
         <v>25</v>
       </c>
       <c r="B6" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C6" t="s">
         <v>25</v>
       </c>
       <c r="D6" t="s">
-        <v>46</v>
+        <v>26</v>
       </c>
       <c r="E6">
         <v>0.01</v>
@@ -1308,19 +1312,19 @@
         <v>25</v>
       </c>
       <c r="B7" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="C7" t="s">
         <v>25</v>
       </c>
       <c r="D7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E7">
         <v>3</v>
       </c>
       <c r="F7" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="G7" t="s">
         <v>0</v>
@@ -1331,13 +1335,13 @@
         <v>25</v>
       </c>
       <c r="B8" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="C8" t="s">
         <v>25</v>
       </c>
       <c r="D8" t="s">
-        <v>46</v>
+        <v>26</v>
       </c>
       <c r="E8">
         <v>0.78</v>
@@ -1351,6 +1355,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
adds exchange type column
</commit_message>
<xml_diff>
--- a/import_test.xlsx
+++ b/import_test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rhanes\GitHub\autoBW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{749F237C-8724-4468-9D3E-FFE8CB80216B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58F1B1A7-DDAF-44CD-BA5E-FC6506A56EAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28845" yWindow="2625" windowWidth="16155" windowHeight="12765" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29295" yWindow="4710" windowWidth="14775" windowHeight="12435" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Create Activities" sheetId="5" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="55">
   <si>
     <t>US</t>
   </si>
@@ -192,6 +192,12 @@
   </si>
   <si>
     <t>activity_location</t>
+  </si>
+  <si>
+    <t>exchange_type</t>
+  </si>
+  <si>
+    <t>technosphere</t>
   </si>
 </sst>
 </file>
@@ -1038,7 +1044,7 @@
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1162,10 +1168,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB2043D1-6EE9-43E0-B324-EF1E0EADF96E}">
-  <dimension ref="A1:N9"/>
+  <dimension ref="A1:O9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1178,10 +1184,10 @@
     <col min="6" max="6" width="40" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="34.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="34.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>49</v>
       </c>
@@ -1210,14 +1216,17 @@
         <v>51</v>
       </c>
       <c r="J1" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="K1" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="K1" s="1"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O1" s="1"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -1242,8 +1251,11 @@
       <c r="I2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>25</v>
       </c>
@@ -1268,8 +1280,11 @@
       <c r="I3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>25</v>
       </c>
@@ -1294,8 +1309,11 @@
       <c r="I4" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -1320,8 +1338,11 @@
       <c r="I5" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -1346,8 +1367,11 @@
       <c r="I6" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>25</v>
       </c>
@@ -1373,10 +1397,13 @@
         <v>45</v>
       </c>
       <c r="J7" t="s">
+        <v>54</v>
+      </c>
+      <c r="K7" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -1401,8 +1428,11 @@
       <c r="I8" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -1426,6 +1456,9 @@
       </c>
       <c r="I9" t="s">
         <v>0</v>
+      </c>
+      <c r="J9" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adds Copy Activities sheet
</commit_message>
<xml_diff>
--- a/import_test.xlsx
+++ b/import_test.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rhanes\GitHub\autoBW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58F1B1A7-DDAF-44CD-BA5E-FC6506A56EAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{144FA2DC-8797-4325-B4C6-907A5D3E21E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29295" yWindow="4710" windowWidth="14775" windowHeight="12435" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28965" yWindow="3150" windowWidth="15945" windowHeight="12045" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Create Activities" sheetId="5" r:id="rId1"/>
-    <sheet name="Add Exchanges" sheetId="4" r:id="rId2"/>
-    <sheet name="Delete Exchanges" sheetId="3" r:id="rId3"/>
+    <sheet name="Copy Activities" sheetId="6" r:id="rId2"/>
+    <sheet name="Add Exchanges" sheetId="4" r:id="rId3"/>
+    <sheet name="Delete Exchanges" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="49">
   <si>
     <t>US</t>
   </si>
@@ -41,24 +42,6 @@
     <t>kg</t>
   </si>
   <si>
-    <t>Exchange Reference Code</t>
-  </si>
-  <si>
-    <t>Exchange Database</t>
-  </si>
-  <si>
-    <t>Database</t>
-  </si>
-  <si>
-    <t>Activity Name</t>
-  </si>
-  <si>
-    <t>Activity Reference Code</t>
-  </si>
-  <si>
-    <t>Exchange Name</t>
-  </si>
-  <si>
     <t>ecoinvent 3.7.1 consequential</t>
   </si>
   <si>
@@ -110,9 +93,6 @@
     <t>43251df807f82a95b6c475078e4ba12c</t>
   </si>
   <si>
-    <t>newdb</t>
-  </si>
-  <si>
     <t>2-Methyl pentane, from chemistry, at plant</t>
   </si>
   <si>
@@ -198,6 +178,9 @@
   </si>
   <si>
     <t>technosphere</t>
+  </si>
+  <si>
+    <t>source_database</t>
   </si>
 </sst>
 </file>
@@ -1043,8 +1026,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{277CB9D4-0D4C-4491-B6C5-72355C9F8902}">
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1062,42 +1045,39 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="B1" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="C1" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="D1" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="E1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
         <v>29</v>
       </c>
-      <c r="F1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G1" t="s">
-        <v>52</v>
-      </c>
-      <c r="H1" t="s">
-        <v>31</v>
-      </c>
-      <c r="I1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" t="s">
-        <v>36</v>
-      </c>
       <c r="C2" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -1116,14 +1096,11 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>25</v>
-      </c>
       <c r="B3" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="C3" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -1139,20 +1116,17 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>25</v>
-      </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="G4" t="s">
         <v>0</v>
@@ -1167,11 +1141,53 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C672BCA2-5B17-4648-9C3C-2F437DABBC60}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB2043D1-6EE9-43E0-B324-EF1E0EADF96E}">
   <dimension ref="A1:O9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1179,47 +1195,48 @@
     <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="32" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="40" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="34.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
@@ -1227,20 +1244,14 @@
       <c r="O1" s="1"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" t="s">
-        <v>25</v>
-      </c>
       <c r="C2" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="E2" t="s">
         <v>0</v>
       </c>
       <c r="F2" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="G2">
         <v>0.8</v>
@@ -1252,82 +1263,64 @@
         <v>0</v>
       </c>
       <c r="J2" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B3" t="s">
-        <v>25</v>
-      </c>
       <c r="C3" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="E3" t="s">
         <v>0</v>
       </c>
       <c r="F3" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="G3">
         <v>0.1</v>
       </c>
       <c r="H3" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="I3" t="s">
         <v>0</v>
       </c>
       <c r="J3" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B4" t="s">
-        <v>25</v>
-      </c>
       <c r="C4" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="E4" t="s">
         <v>0</v>
       </c>
       <c r="F4" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="G4">
         <v>4</v>
       </c>
       <c r="H4" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="I4" t="s">
         <v>0</v>
       </c>
       <c r="J4" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B5" t="s">
-        <v>25</v>
-      </c>
       <c r="C5" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="E5" t="s">
         <v>0</v>
       </c>
       <c r="F5" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="G5">
         <v>0.2</v>
@@ -1339,24 +1332,18 @@
         <v>0</v>
       </c>
       <c r="J5" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B6" t="s">
-        <v>25</v>
-      </c>
       <c r="C6" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="E6" t="s">
         <v>0</v>
       </c>
       <c r="F6" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="G6">
         <v>0.01</v>
@@ -1368,85 +1355,70 @@
         <v>0</v>
       </c>
       <c r="J6" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>25</v>
-      </c>
       <c r="B7" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="C7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" t="s">
+        <v>0</v>
+      </c>
+      <c r="F7" t="s">
         <v>36</v>
-      </c>
-      <c r="E7" t="s">
-        <v>0</v>
-      </c>
-      <c r="F7" t="s">
-        <v>43</v>
       </c>
       <c r="G7">
         <v>0.5</v>
       </c>
       <c r="H7" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="I7" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="J7" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="K7" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B8" t="s">
-        <v>25</v>
-      </c>
       <c r="C8" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="E8" t="s">
         <v>0</v>
       </c>
       <c r="F8" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="G8">
         <v>3</v>
       </c>
       <c r="H8" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="I8" t="s">
         <v>0</v>
       </c>
       <c r="J8" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9" t="s">
-        <v>25</v>
-      </c>
       <c r="C9" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="E9" t="s">
         <v>0</v>
       </c>
       <c r="F9" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="G9">
         <v>0.78</v>
@@ -1458,7 +1430,7 @@
         <v>0</v>
       </c>
       <c r="J9" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -1467,12 +1439,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0948324-ADD0-429A-AD05-3510BCB3C5ED}">
   <dimension ref="A1:Q5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1487,22 +1459,22 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>4</v>
+        <v>42</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>6</v>
+        <v>33</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>43</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>2</v>
+        <v>41</v>
       </c>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
@@ -1518,82 +1490,82 @@
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E2" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" t="s">
-        <v>14</v>
-      </c>
       <c r="F3" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E4" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="F4" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D5" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E5" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="F5" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
partial reformat per black
</commit_message>
<xml_diff>
--- a/import_test.xlsx
+++ b/import_test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rhanes\GitHub\autoBW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{144FA2DC-8797-4325-B4C6-907A5D3E21E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{604311D3-54F1-4C21-A04A-E199190D13F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28965" yWindow="3150" windowWidth="15945" windowHeight="12045" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28905" yWindow="1365" windowWidth="15960" windowHeight="14955" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Create Activities" sheetId="5" r:id="rId1"/>
@@ -1145,7 +1145,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
begin refactor; broken at data_manager
</commit_message>
<xml_diff>
--- a/import_test.xlsx
+++ b/import_test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rhanes\GitHub\autoBW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{604311D3-54F1-4C21-A04A-E199190D13F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C5D6F54-1B63-4895-933F-1EBEC2DEC38C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28905" yWindow="1365" windowWidth="15960" windowHeight="14955" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29715" yWindow="4020" windowWidth="16215" windowHeight="14955" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Create Activities" sheetId="5" r:id="rId1"/>
@@ -1026,8 +1026,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{277CB9D4-0D4C-4491-B6C5-72355C9F8902}">
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1144,7 +1144,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C672BCA2-5B17-4648-9C3C-2F437DABBC60}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
minimal updates to file for testing error handling
</commit_message>
<xml_diff>
--- a/import_test.xlsx
+++ b/import_test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rhanes\GitHub\autoBW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C5D6F54-1B63-4895-933F-1EBEC2DEC38C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{786736D6-51B0-4BEE-98A1-34497D8F724C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29715" yWindow="4020" windowWidth="16215" windowHeight="14955" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10935" yWindow="690" windowWidth="16215" windowHeight="14955" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Create Activities" sheetId="5" r:id="rId1"/>
@@ -1026,7 +1026,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{277CB9D4-0D4C-4491-B6C5-72355C9F8902}">
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
@@ -1144,7 +1144,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C672BCA2-5B17-4648-9C3C-2F437DABBC60}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
updates import file and testing template
</commit_message>
<xml_diff>
--- a/import_test.xlsx
+++ b/import_test.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rhanes\GitHub\autoBW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{786736D6-51B0-4BEE-98A1-34497D8F724C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25599EB2-BCEE-402C-999F-950A7D702FC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10935" yWindow="690" windowWidth="16215" windowHeight="14955" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29370" yWindow="-6480" windowWidth="15630" windowHeight="11835" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Create Activities" sheetId="5" r:id="rId1"/>
     <sheet name="Copy Activities" sheetId="6" r:id="rId2"/>
-    <sheet name="Add Exchanges" sheetId="4" r:id="rId3"/>
-    <sheet name="Delete Exchanges" sheetId="3" r:id="rId4"/>
+    <sheet name="Delete Exchanges" sheetId="3" r:id="rId3"/>
+    <sheet name="Add Exchanges" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="43">
   <si>
     <t>US</t>
   </si>
@@ -42,57 +42,12 @@
     <t>kg</t>
   </si>
   <si>
-    <t>ecoinvent 3.7.1 consequential</t>
-  </si>
-  <si>
-    <t>lubricating oil production</t>
-  </si>
-  <si>
-    <t>1e9857fe7e9c88bbbaff87b7fd322d4e</t>
-  </si>
-  <si>
-    <t>market group for diesel</t>
-  </si>
-  <si>
-    <t>market for steel, chromium steel 18/8</t>
-  </si>
-  <si>
-    <t>186e19fa6465514ebe6243b36382520a</t>
-  </si>
-  <si>
-    <t>transport, freight train</t>
-  </si>
-  <si>
-    <t>1f54ef3533e0ca95122c1f869428c541</t>
-  </si>
-  <si>
-    <t>cement production, Portland</t>
-  </si>
-  <si>
-    <t>ffd6836cd82ac339b36616cbb9dd6ff4</t>
-  </si>
-  <si>
-    <t>market for gypsum, mineral</t>
-  </si>
-  <si>
-    <t>0733b2583ae87bebc1bb4a64798ade38</t>
-  </si>
-  <si>
     <t>market for electricity, medium voltage</t>
   </si>
   <si>
     <t>electric grid mix</t>
   </si>
   <si>
-    <t>04b818d7946b8689c96aaea50d6a076f</t>
-  </si>
-  <si>
-    <t>market for transmission network, electricity, medium voltage</t>
-  </si>
-  <si>
-    <t>43251df807f82a95b6c475078e4ba12c</t>
-  </si>
-  <si>
     <t>2-Methyl pentane, from chemistry, at plant</t>
   </si>
   <si>
@@ -181,6 +136,33 @@
   </si>
   <si>
     <t>source_database</t>
+  </si>
+  <si>
+    <t>activity_type</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>destination_database</t>
+  </si>
+  <si>
+    <t>nrel psh</t>
+  </si>
+  <si>
+    <t>ecoinvent3.8 cut-off</t>
+  </si>
+  <si>
+    <t>tap water production, underground water without treatment</t>
+  </si>
+  <si>
+    <t>903957dbaf8147dda6c17296323caa3e</t>
+  </si>
+  <si>
+    <t>a3f826ed5f0817aeb0e82dea83709f7c</t>
+  </si>
+  <si>
+    <t>delete CA-QC med electric and replace with US</t>
   </si>
 </sst>
 </file>
@@ -664,10 +646,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
@@ -1024,114 +1005,130 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{277CB9D4-0D4C-4491-B6C5-72355C9F8902}">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="40" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" customWidth="1"/>
+    <col min="3" max="3" width="39.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="B1" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C1" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D1" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="E1" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="F1" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="G1" t="s">
-        <v>45</v>
+        <v>8</v>
       </c>
       <c r="H1" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="I1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="J1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2">
         <v>1</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>1</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>2</v>
       </c>
-      <c r="G2" t="s">
-        <v>0</v>
-      </c>
-      <c r="H2">
+      <c r="H2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I2">
         <v>0.1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D3">
+        <v>16</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3">
         <v>1</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>1</v>
       </c>
-      <c r="G3" t="s">
-        <v>0</v>
-      </c>
-      <c r="H3">
+      <c r="H3" t="s">
+        <v>0</v>
+      </c>
+      <c r="I3">
         <v>0.1</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="C4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4">
         <v>1</v>
       </c>
-      <c r="E4" t="s">
-        <v>28</v>
-      </c>
-      <c r="G4" t="s">
-        <v>0</v>
-      </c>
-      <c r="H4">
+      <c r="F4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" t="s">
+        <v>0</v>
+      </c>
+      <c r="I4">
         <v>0.1</v>
       </c>
     </row>
@@ -1142,10 +1139,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C672BCA2-5B17-4648-9C3C-2F437DABBC60}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1155,26 +1152,46 @@
     <col min="3" max="3" width="34.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="B1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" t="s">
         <v>40</v>
       </c>
-      <c r="C1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C2" t="s">
-        <v>39</v>
+      <c r="D3" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1183,12 +1200,87 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0948324-ADD0-429A-AD05-3510BCB3C5ED}">
+  <dimension ref="A1:Q2"/>
+  <sheetViews>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="56.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="34" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB2043D1-6EE9-43E0-B324-EF1E0EADF96E}">
   <dimension ref="A1:O9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
-    </sheetView>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1206,37 +1298,37 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="F1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="D1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>41</v>
       </c>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
@@ -1245,13 +1337,13 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="E2" t="s">
         <v>0</v>
       </c>
       <c r="F2" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="G2">
         <v>0.8</v>
@@ -1263,64 +1355,64 @@
         <v>0</v>
       </c>
       <c r="J2" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="E3" t="s">
         <v>0</v>
       </c>
       <c r="F3" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="G3">
         <v>0.1</v>
       </c>
       <c r="H3" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="I3" t="s">
         <v>0</v>
       </c>
       <c r="J3" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="E4" t="s">
         <v>0</v>
       </c>
       <c r="F4" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="G4">
         <v>4</v>
       </c>
       <c r="H4" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="I4" t="s">
         <v>0</v>
       </c>
       <c r="J4" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="E5" t="s">
         <v>0</v>
       </c>
       <c r="F5" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="G5">
         <v>0.2</v>
@@ -1332,18 +1424,18 @@
         <v>0</v>
       </c>
       <c r="J5" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="E6" t="s">
         <v>0</v>
       </c>
       <c r="F6" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="G6">
         <v>0.01</v>
@@ -1355,70 +1447,70 @@
         <v>0</v>
       </c>
       <c r="J6" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="C7" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="E7" t="s">
         <v>0</v>
       </c>
       <c r="F7" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="G7">
         <v>0.5</v>
       </c>
       <c r="H7" t="s">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="I7" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="J7" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="K7" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="E8" t="s">
         <v>0</v>
       </c>
       <c r="F8" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="G8">
         <v>3</v>
       </c>
       <c r="H8" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="I8" t="s">
         <v>0</v>
       </c>
       <c r="J8" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="E9" t="s">
         <v>0</v>
       </c>
       <c r="F9" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="G9">
         <v>0.78</v>
@@ -1430,146 +1522,11 @@
         <v>0</v>
       </c>
       <c r="J9" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0948324-ADD0-429A-AD05-3510BCB3C5ED}">
-  <dimension ref="A1:Q5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="28" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="56.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="34" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" t="s">
-        <v>2</v>
-      </c>
-      <c r="E5" t="s">
-        <v>17</v>
-      </c>
-      <c r="F5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>